<commit_message>
This is a major update for AP4. Moving to a Queued based state machine
</commit_message>
<xml_diff>
--- a/NI-2010/Trunk/Hybrid Water Heater/Macros/UEF/Example Data/FHR/FHR Check Data.xlsx
+++ b/NI-2010/Trunk/Hybrid Water Heater/Macros/UEF/Example Data/FHR/FHR Check Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TechnologyLab\NI-2010\Trunk\Hybrid Water Heater\Macros\UEF\Example Data\FHR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8B92C10-7D78-4973-8A58-1FAEAFD087A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F84908FF-65B5-4B0A-87D5-1BB5A84FB55C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8052" yWindow="1596" windowWidth="12072" windowHeight="10788" xr2:uid="{79FF0471-CA74-4CE7-A257-097B3DEA5E2F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{79FF0471-CA74-4CE7-A257-097B3DEA5E2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
   <si>
     <t>TR Number</t>
   </si>
@@ -44,31 +44,88 @@
     <t>20WS1064</t>
   </si>
   <si>
-    <t>20WS1095</t>
-  </si>
-  <si>
-    <t>21WS1094</t>
-  </si>
-  <si>
-    <t>21WS1095</t>
-  </si>
-  <si>
     <t>Macro Rating (Gallons)</t>
   </si>
   <si>
-    <t>Time Stamp</t>
-  </si>
-  <si>
-    <t>14_33</t>
-  </si>
-  <si>
-    <t>9_45</t>
+    <t>TR_AWP20WS10184_Lab_ID_20WS1064_Md_GG50T12BXR01 08_59FHR</t>
+  </si>
+  <si>
+    <t>Partial Bonus Draw?</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>TR_AWP21WS10211_Lab_ID_21WS1095_Model_GG50S08_Date_06_10_2021_Time_09_45FHR_File0_Data</t>
+  </si>
+  <si>
+    <t>20WS1095-Run1</t>
+  </si>
+  <si>
+    <t>21WS1095-Run 2</t>
+  </si>
+  <si>
+    <t>TR_AWP21WS10211_Lab_ID_21WS1095_Model_GG50S08_Date_06_10_2021_Time_14_33FHR_File1_Data</t>
+  </si>
+  <si>
+    <t>Filename</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>24WS1597</t>
+  </si>
+  <si>
+    <t>TR_AWP24WS10416_Lab_ID_24WS1597_Model_PH50S10BNY_Date_09_27_2024_Time_21_581st Hour Rating_File1_Data</t>
+  </si>
+  <si>
+    <t>TR_AWP24WS10416_Lab_ID_24WS1595_Model_PH50S10BNY_Date_09_24_2024_Time_14_051st Hour Rating_File0_Data</t>
+  </si>
+  <si>
+    <t>24WS1595</t>
+  </si>
+  <si>
+    <t>Difference</t>
+  </si>
+  <si>
+    <t>TR_sheldon_energy_50g_top_t_p_Lab_ID_GZ600462X_Model_GE50S08BAM01 _Date_10_08_2024_Time_16_30FHR_</t>
+  </si>
+  <si>
+    <t>GE50S08BAM01</t>
+  </si>
+  <si>
+    <t>TR_AWP24WS10416_Lab_ID_24WS1596_Model_PH50S10BNY_Date_10_22_2024_Time_18_311st Hour Rating_</t>
+  </si>
+  <si>
+    <t>Data Set 4</t>
+  </si>
+  <si>
+    <t>TR_AWP24WS10429_Lab_ID_24WS1687_Model_PJ50S10FPY_Date_11_21_2024_Time_13_031st Hour Rating_File0_Data</t>
+  </si>
+  <si>
+    <t>Data Set 5</t>
+  </si>
+  <si>
+    <t>Version 41</t>
+  </si>
+  <si>
+    <t>Version Difference</t>
+  </si>
+  <si>
+    <t>Version 42 FHR (Gallons)</t>
+  </si>
+  <si>
+    <t>Version 41 FHR (Gallons)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -78,15 +135,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -94,12 +157,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -118,9 +201,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -158,7 +241,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -264,7 +347,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -406,7 +489,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -414,72 +497,369 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92A76E7E-80E1-4E8E-8B84-5472FB40E3F3}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.109375" customWidth="1"/>
-    <col min="3" max="3" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="108.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.42578125" customWidth="1"/>
+    <col min="5" max="6" width="23" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="3">
+        <v>85.646000000000001</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="2">
+        <v>85.646000000000001</v>
+      </c>
+      <c r="F2" s="2">
+        <f>E2-C2</f>
+        <v>0</v>
+      </c>
+      <c r="G2" s="2">
+        <v>85.856999999999999</v>
+      </c>
+      <c r="H2" s="2">
+        <f>E2-G2</f>
+        <v>-0.21099999999999852</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="C3" s="3">
+        <v>86.947500000000005</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2">
-        <v>85.5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5">
-        <v>81.16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="E3" s="2">
+        <v>86.947500000000005</v>
+      </c>
+      <c r="F3" s="2">
+        <f t="shared" ref="F3:F9" si="0">E3-C3</f>
+        <v>0</v>
+      </c>
+      <c r="G3" s="2">
+        <v>87.0565</v>
+      </c>
+      <c r="H3" s="2">
+        <f t="shared" ref="H3:H9" si="1">E3-G3</f>
+        <v>-0.10899999999999466</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D6">
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="3">
+        <v>81.051599999999993</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="2">
+        <v>81.051599999999993</v>
+      </c>
+      <c r="F4" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G4" s="2">
+        <v>80.939499999999995</v>
+      </c>
+      <c r="H4" s="2">
+        <f t="shared" si="1"/>
+        <v>0.11209999999999809</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="3">
+        <v>74.319999999999993</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="2">
+        <v>74.319999999999993</v>
+      </c>
+      <c r="F5" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G5" s="2">
+        <v>74.489000000000004</v>
+      </c>
+      <c r="H5" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.16900000000001114</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="3">
+        <v>75.23</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="2">
+        <v>75.227000000000004</v>
+      </c>
+      <c r="F6" s="2">
+        <f t="shared" si="0"/>
+        <v>-3.0000000000001137E-3</v>
+      </c>
+      <c r="G6" s="2">
+        <v>75.400999999999996</v>
+      </c>
+      <c r="H6" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.17399999999999238</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="3">
+        <v>72.918000000000006</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="2">
+        <v>72.918000000000006</v>
+      </c>
+      <c r="F7" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G7" s="2">
+        <v>73.278999999999996</v>
+      </c>
+      <c r="H7" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.36099999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="3">
+        <v>75.293999999999997</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="2">
+        <v>75.293999999999997</v>
+      </c>
+      <c r="F8" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G8" s="2">
+        <v>75.555999999999997</v>
+      </c>
+      <c r="H8" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.26200000000000045</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="5">
+        <v>59.203000000000003</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="2">
+        <v>59.203000000000003</v>
+      </c>
+      <c r="F9" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G9" s="2">
+        <v>59.215000000000003</v>
+      </c>
+      <c r="H9" s="2">
+        <f t="shared" si="1"/>
+        <v>-1.2000000000000455E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E14" s="2">
+        <v>85.646000000000001</v>
+      </c>
+      <c r="F14" s="2">
+        <v>85.856999999999999</v>
+      </c>
+      <c r="G14" s="2">
+        <v>-0.21099999999999852</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E15" s="2">
+        <v>86.947500000000005</v>
+      </c>
+      <c r="F15" s="2">
         <v>87.0565</v>
+      </c>
+      <c r="G15" s="2">
+        <v>-0.10899999999999466</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E16" s="2">
+        <v>81.051599999999993</v>
+      </c>
+      <c r="F16" s="2">
+        <v>80.939499999999995</v>
+      </c>
+      <c r="G16" s="2">
+        <v>0.11209999999999809</v>
+      </c>
+    </row>
+    <row r="17" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E17" s="2">
+        <v>74.319999999999993</v>
+      </c>
+      <c r="F17" s="2">
+        <v>74.489000000000004</v>
+      </c>
+      <c r="G17" s="2">
+        <v>-0.16900000000001114</v>
+      </c>
+    </row>
+    <row r="18" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E18" s="2">
+        <v>75.227000000000004</v>
+      </c>
+      <c r="F18" s="2">
+        <v>75.400999999999996</v>
+      </c>
+      <c r="G18" s="2">
+        <v>-0.17399999999999238</v>
+      </c>
+    </row>
+    <row r="19" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E19" s="2">
+        <v>72.918000000000006</v>
+      </c>
+      <c r="F19" s="2">
+        <v>73.278999999999996</v>
+      </c>
+      <c r="G19" s="2">
+        <v>-0.36099999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E20" s="2">
+        <v>75.293999999999997</v>
+      </c>
+      <c r="F20" s="2">
+        <v>75.555999999999997</v>
+      </c>
+      <c r="G20" s="2">
+        <v>-0.26200000000000045</v>
+      </c>
+    </row>
+    <row r="21" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E21" s="2">
+        <v>59.203000000000003</v>
+      </c>
+      <c r="F21" s="2">
+        <v>59.215000000000003</v>
+      </c>
+      <c r="G21" s="2">
+        <v>-1.2000000000000455E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FHR Data Check excel files
</commit_message>
<xml_diff>
--- a/NI-2010/Trunk/Hybrid Water Heater/Macros/UEF/Example Data/FHR/FHR Check Data.xlsx
+++ b/NI-2010/Trunk/Hybrid Water Heater/Macros/UEF/Example Data/FHR/FHR Check Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TechnologyLab\NI-2010\Trunk\Hybrid Water Heater\Macros\UEF\Example Data\FHR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F84908FF-65B5-4B0A-87D5-1BB5A84FB55C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A7D7A19-7E30-4544-BF6B-C10F4944F3C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{79FF0471-CA74-4CE7-A257-097B3DEA5E2F}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{79FF0471-CA74-4CE7-A257-097B3DEA5E2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="46">
   <si>
     <t>TR Number</t>
   </si>
@@ -107,16 +107,70 @@
     <t>Data Set 5</t>
   </si>
   <si>
-    <t>Version 41</t>
-  </si>
-  <si>
-    <t>Version Difference</t>
-  </si>
-  <si>
-    <t>Version 42 FHR (Gallons)</t>
-  </si>
-  <si>
-    <t>Version 41 FHR (Gallons)</t>
+    <t>FHD Mistake</t>
+  </si>
+  <si>
+    <t>FHD Mistake 2</t>
+  </si>
+  <si>
+    <t>FHD Mistake 3</t>
+  </si>
+  <si>
+    <t>TR_AWP25WS10441_Lab_ID_25WS1753_Model_GE50S08BAY_Date_02_19_2025_Time_12_191st Hour Rating_File0_Data</t>
+  </si>
+  <si>
+    <t>TR_AWP25WS10445_Lab_ID_25WS1802_Model_PH65S10BNY_Date_03_19_2025_Time_20_541st Hour Rating_File1_Data</t>
+  </si>
+  <si>
+    <t>TR_AWP25WS10450_Lab_ID_25WS1804_Model_PK65S10FNY_Date_03_28_2025_Time_08_401st Hour Rating_File0_Data</t>
+  </si>
+  <si>
+    <t>TR_AWP25WS10443_Lab_ID_25WS1794_Model_PJ65S10FPY_Date_03_12_2025_Time_14_071st Hour Rating_</t>
+  </si>
+  <si>
+    <t>25WS1794</t>
+  </si>
+  <si>
+    <t>25WS1795</t>
+  </si>
+  <si>
+    <t>TR_AWP25WS10443_Lab_ID_25WS1795_Model_PF65S10FPY_Date_03_04_2025_Time_14_301st Hour Rating_</t>
+  </si>
+  <si>
+    <t>TR_AWP25WS10444_Lab_ID_25WS1799_Model_PH65S10BPY_Date_03_04_2025_Time_14_161st Hour Rating_File2_Data</t>
+  </si>
+  <si>
+    <t>25WS1799</t>
+  </si>
+  <si>
+    <t>25WS1802</t>
+  </si>
+  <si>
+    <t>TR_AWP25WS10450_Lab_ID_25WS1802_Model_PK65S10FNY_Date_04_03_2025_Time_15_031st Hour Rating_File2_Data</t>
+  </si>
+  <si>
+    <t>TR_AWP25WS10447_Lab_ID_25WS1810_Model_PF80S10FPY_Date_04_14_2025_Time_07_061st Hour Rating_</t>
+  </si>
+  <si>
+    <t>25WS1810</t>
+  </si>
+  <si>
+    <t>TR_AWP25WS10448_Lab_ID_25WS1814_Model_PH80S10BPY_Date_04_11_2025_Time_21_551st Hour Rating_File1_Data</t>
+  </si>
+  <si>
+    <t>25WS1814</t>
+  </si>
+  <si>
+    <t>25WS1807</t>
+  </si>
+  <si>
+    <t>TR_AWP25WS10452_Lab_ID_25WS1807_Model_PK80S10FNY_Date_04_05_2025_Time_21_291st Hour Rating_File2_Data</t>
+  </si>
+  <si>
+    <t>TR_AWP25WS10446_Lab_ID_25WS1806_Model_PH80S10FBNY_Date_03_25_2025_Time_17_331st Hour Rating_File1_Data</t>
+  </si>
+  <si>
+    <t>25WS1806</t>
   </si>
 </sst>
 </file>
@@ -149,7 +203,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -172,17 +226,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -497,10 +567,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92A76E7E-80E1-4E8E-8B84-5472FB40E3F3}">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -526,18 +596,14 @@
       <c r="D1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -552,20 +618,15 @@
       <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="5">
         <v>85.646000000000001</v>
       </c>
       <c r="F2" s="2">
         <f>E2-C2</f>
         <v>0</v>
       </c>
-      <c r="G2" s="2">
-        <v>85.856999999999999</v>
-      </c>
-      <c r="H2" s="2">
-        <f>E2-G2</f>
-        <v>-0.21099999999999852</v>
-      </c>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -580,20 +641,15 @@
       <c r="D3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="5">
         <v>86.947500000000005</v>
       </c>
       <c r="F3" s="2">
-        <f t="shared" ref="F3:F9" si="0">E3-C3</f>
-        <v>0</v>
-      </c>
-      <c r="G3" s="2">
-        <v>87.0565</v>
-      </c>
-      <c r="H3" s="2">
-        <f t="shared" ref="H3:H9" si="1">E3-G3</f>
-        <v>-0.10899999999999466</v>
-      </c>
+        <f t="shared" ref="F3:F20" si="0">E3-C3</f>
+        <v>0</v>
+      </c>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -608,20 +664,15 @@
       <c r="D4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="2">
-        <v>81.051599999999993</v>
+      <c r="E4" s="5">
+        <v>81.078400000000002</v>
       </c>
       <c r="F4" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G4" s="2">
-        <v>80.939499999999995</v>
-      </c>
-      <c r="H4" s="2">
-        <f t="shared" si="1"/>
-        <v>0.11209999999999809</v>
-      </c>
+        <v>2.6800000000008595E-2</v>
+      </c>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -636,20 +687,15 @@
       <c r="D5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="5">
         <v>74.319999999999993</v>
       </c>
       <c r="F5" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G5" s="2">
-        <v>74.489000000000004</v>
-      </c>
-      <c r="H5" s="2">
-        <f t="shared" si="1"/>
-        <v>-0.16900000000001114</v>
-      </c>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
@@ -664,20 +710,15 @@
       <c r="D6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="5">
         <v>75.227000000000004</v>
       </c>
       <c r="F6" s="2">
         <f t="shared" si="0"/>
         <v>-3.0000000000001137E-3</v>
       </c>
-      <c r="G6" s="2">
-        <v>75.400999999999996</v>
-      </c>
-      <c r="H6" s="2">
-        <f t="shared" si="1"/>
-        <v>-0.17399999999999238</v>
-      </c>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
@@ -692,20 +733,15 @@
       <c r="D7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="5">
         <v>72.918000000000006</v>
       </c>
       <c r="F7" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G7" s="2">
-        <v>73.278999999999996</v>
-      </c>
-      <c r="H7" s="2">
-        <f t="shared" si="1"/>
-        <v>-0.36099999999999</v>
-      </c>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
@@ -720,147 +756,291 @@
       <c r="D8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="5">
         <v>75.293999999999997</v>
       </c>
       <c r="F8" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G8" s="2">
-        <v>75.555999999999997</v>
-      </c>
-      <c r="H8" s="2">
-        <f t="shared" si="1"/>
-        <v>-0.26200000000000045</v>
-      </c>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="3">
         <v>59.203000000000003</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="5">
         <v>59.203000000000003</v>
       </c>
       <c r="F9" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G9" s="2">
-        <v>59.215000000000003</v>
-      </c>
-      <c r="H9" s="2">
-        <f t="shared" si="1"/>
-        <v>-1.2000000000000455E-2</v>
-      </c>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="3">
+        <v>74.22</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="2">
+        <v>74.215000000000003</v>
+      </c>
+      <c r="F10" s="3">
+        <f>E10-C10</f>
+        <v>-4.9999999999954525E-3</v>
+      </c>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="3">
+        <v>85.36</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="2">
+        <v>85.355000000000004</v>
+      </c>
+      <c r="F11" s="2">
+        <f t="shared" si="0"/>
+        <v>-4.9999999999954525E-3</v>
+      </c>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="3">
+        <v>67.576999999999998</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="2">
+        <v>67.577299999999994</v>
+      </c>
+      <c r="F12" s="2">
+        <f t="shared" si="0"/>
+        <v>2.9999999999574811E-4</v>
+      </c>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E13" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="A13" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="7">
+        <v>77.831000000000003</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="2">
+        <v>77.831000000000003</v>
+      </c>
+      <c r="F13" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E14" s="2">
-        <v>85.646000000000001</v>
-      </c>
-      <c r="F14" s="2">
-        <v>85.856999999999999</v>
-      </c>
-      <c r="G14" s="2">
-        <v>-0.21099999999999852</v>
-      </c>
+      <c r="A14" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="7">
+        <v>77.823999999999998</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" s="6">
+        <v>77.823999999999998</v>
+      </c>
+      <c r="F14" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E15" s="2">
-        <v>86.947500000000005</v>
-      </c>
-      <c r="F15" s="2">
-        <v>87.0565</v>
-      </c>
-      <c r="G15" s="2">
-        <v>-0.10899999999999466</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E16" s="2">
-        <v>81.051599999999993</v>
-      </c>
-      <c r="F16" s="2">
-        <v>80.939499999999995</v>
-      </c>
-      <c r="G16" s="2">
-        <v>0.11209999999999809</v>
-      </c>
-    </row>
-    <row r="17" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E17" s="2">
-        <v>74.319999999999993</v>
-      </c>
-      <c r="F17" s="2">
-        <v>74.489000000000004</v>
-      </c>
-      <c r="G17" s="2">
-        <v>-0.16900000000001114</v>
-      </c>
-    </row>
-    <row r="18" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E18" s="2">
-        <v>75.227000000000004</v>
-      </c>
-      <c r="F18" s="2">
-        <v>75.400999999999996</v>
-      </c>
-      <c r="G18" s="2">
-        <v>-0.17399999999999238</v>
-      </c>
-    </row>
-    <row r="19" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E19" s="2">
-        <v>72.918000000000006</v>
-      </c>
-      <c r="F19" s="2">
-        <v>73.278999999999996</v>
-      </c>
-      <c r="G19" s="2">
-        <v>-0.36099999999999</v>
-      </c>
-    </row>
-    <row r="20" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E20" s="2">
-        <v>75.293999999999997</v>
-      </c>
-      <c r="F20" s="2">
-        <v>75.555999999999997</v>
-      </c>
-      <c r="G20" s="2">
-        <v>-0.26200000000000045</v>
-      </c>
-    </row>
-    <row r="21" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E21" s="2">
-        <v>59.203000000000003</v>
-      </c>
-      <c r="F21" s="2">
-        <v>59.215000000000003</v>
-      </c>
-      <c r="G21" s="2">
-        <v>-1.2000000000000455E-2</v>
-      </c>
+      <c r="A15" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="7">
+        <v>87.028000000000006</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="6">
+        <v>87.028000000000006</v>
+      </c>
+      <c r="F15" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="7">
+        <v>64.852999999999994</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" s="6">
+        <v>64.852900000000005</v>
+      </c>
+      <c r="F16" s="6">
+        <f t="shared" si="0"/>
+        <v>-9.9999999989108801E-5</v>
+      </c>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="7">
+        <v>94.200999999999993</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="6">
+        <v>94.200999999999993</v>
+      </c>
+      <c r="F17" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="7">
+        <v>101.06</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" s="6">
+        <v>101.06</v>
+      </c>
+      <c r="F18" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="7">
+        <v>77.057000000000002</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" s="6">
+        <v>77.057000000000002</v>
+      </c>
+      <c r="F19" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" s="7">
+        <v>100.973</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" s="6">
+        <v>100.973</v>
+      </c>
+      <c r="F20" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>